<commit_message>
Fixed Production Date and Days in Shop
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -527,7 +527,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -558,7 +558,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-07-28</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2024-07-20</t>
+          <t>2024-08-02</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -638,46 +638,46 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>2024-03-14</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Donovan Gamboa</t>
+          <t>Walter</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>911</t>
+          <t>92020483</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Home</t>
+          <t>Aomdonm</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2024-07-16</t>
+          <t>2024-05-28</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>$500</t>
+          <t>$3920</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Scooby</t>
+          <t>Ansoansoansaonason</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>J8008</t>
+          <t>J99999</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>

</xml_diff>